<commit_message>
Minor changes and added new input scripts
</commit_message>
<xml_diff>
--- a/scripts/data/__index__.xlsx
+++ b/scripts/data/__index__.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\calibrate\optimiser\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unsw-my.sharepoint.com/personal/z5208868_ad_unsw_edu_au/Documents/Desktop/code/moga_neml/scripts/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FEBC61-1C44-487D-B64C-5DBBFC95A2F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="225" yWindow="225" windowWidth="28575" windowHeight="15375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="notes" sheetId="16" r:id="rId1"/>
@@ -1913,13 +1913,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E05C7426-797A-4E08-8D89-586E3BDD972F}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>269</v>
       </c>
@@ -1930,7 +1930,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>270</v>
       </c>
@@ -1950,24 +1950,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72057042-979B-4A98-BA2E-14DCB6564B56}">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" style="8" customWidth="1"/>
-    <col min="3" max="6" width="9.140625" style="3"/>
-    <col min="7" max="7" width="9.140625" style="8"/>
-    <col min="8" max="8" width="9.140625" style="2"/>
-    <col min="9" max="9" width="9.140625" style="3"/>
-    <col min="10" max="10" width="8.5703125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="8.42578125" style="8" customWidth="1"/>
-    <col min="12" max="12" width="25.7109375" style="10" customWidth="1"/>
+    <col min="1" max="1" width="4.453125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7265625" style="8" customWidth="1"/>
+    <col min="3" max="6" width="9.1796875" style="3"/>
+    <col min="7" max="7" width="9.1796875" style="8"/>
+    <col min="8" max="8" width="9.1796875" style="2"/>
+    <col min="9" max="9" width="9.1796875" style="3"/>
+    <col min="10" max="10" width="8.54296875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="8.453125" style="8" customWidth="1"/>
+    <col min="12" max="12" width="25.7265625" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>131</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>132</v>
       </c>
@@ -2040,7 +2040,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>133</v>
       </c>
@@ -2072,7 +2072,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>135</v>
       </c>
@@ -2107,7 +2107,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>137</v>
       </c>
@@ -2139,7 +2139,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>138</v>
       </c>
@@ -2171,7 +2171,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>139</v>
       </c>
@@ -2206,7 +2206,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
         <v>136</v>
       </c>
@@ -2241,7 +2241,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="15" t="s">
         <v>140</v>
       </c>
@@ -2275,7 +2275,7 @@
       </c>
       <c r="L9" s="16"/>
     </row>
-    <row r="10" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>134</v>
       </c>
@@ -2309,7 +2309,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>141</v>
       </c>
@@ -2345,7 +2345,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>142</v>
       </c>
@@ -2379,7 +2379,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>143</v>
       </c>
@@ -2415,7 +2415,7 @@
       </c>
       <c r="L13" s="9"/>
     </row>
-    <row r="14" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>144</v>
       </c>
@@ -2449,7 +2449,7 @@
       </c>
       <c r="L14" s="9"/>
     </row>
-    <row r="15" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>145</v>
       </c>
@@ -2485,7 +2485,7 @@
       </c>
       <c r="L15" s="9"/>
     </row>
-    <row r="16" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>146</v>
       </c>
@@ -2519,7 +2519,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>147</v>
       </c>
@@ -2555,7 +2555,7 @@
       </c>
       <c r="L17" s="9"/>
     </row>
-    <row r="18" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
         <v>148</v>
       </c>
@@ -2589,7 +2589,7 @@
       </c>
       <c r="L18" s="13"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="8" t="s">
         <v>149</v>
       </c>
@@ -2624,7 +2624,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="8" t="s">
         <v>150</v>
       </c>
@@ -2656,7 +2656,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" s="8" t="s">
         <v>151</v>
       </c>
@@ -2691,7 +2691,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" s="8" t="s">
         <v>152</v>
       </c>
@@ -2726,7 +2726,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" s="8" t="s">
         <v>153</v>
       </c>
@@ -2758,7 +2758,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" s="8" t="s">
         <v>154</v>
       </c>
@@ -2793,7 +2793,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="15" t="s">
         <v>155</v>
       </c>
@@ -2838,25 +2838,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9578FDA3-F26E-4E35-80A8-9B064AEAD5AE}">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="2"/>
-    <col min="4" max="7" width="9.140625" style="3"/>
-    <col min="8" max="8" width="9.140625" style="2"/>
-    <col min="9" max="9" width="9.140625" style="3"/>
-    <col min="10" max="10" width="8.5703125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="8.42578125" style="3" customWidth="1"/>
-    <col min="12" max="12" width="25.7109375" style="19" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="22"/>
+    <col min="1" max="1" width="4.54296875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7265625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" style="2"/>
+    <col min="4" max="7" width="9.1796875" style="3"/>
+    <col min="8" max="8" width="9.1796875" style="2"/>
+    <col min="9" max="9" width="9.1796875" style="3"/>
+    <col min="10" max="10" width="8.54296875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="8.453125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="25.7265625" style="19" customWidth="1"/>
+    <col min="13" max="13" width="9.1796875" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>131</v>
       </c>
@@ -2895,7 +2895,7 @@
       </c>
       <c r="M1" s="25"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>156</v>
       </c>
@@ -2927,7 +2927,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>157</v>
       </c>
@@ -2962,7 +2962,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>158</v>
       </c>
@@ -2997,7 +2997,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>159</v>
       </c>
@@ -3029,7 +3029,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="15" t="s">
         <v>160</v>
       </c>
@@ -3066,7 +3066,7 @@
       <c r="L6" s="26"/>
       <c r="M6" s="27"/>
     </row>
-    <row r="7" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>161</v>
       </c>
@@ -3103,7 +3103,7 @@
       <c r="L7" s="20"/>
       <c r="M7" s="21"/>
     </row>
-    <row r="8" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>162</v>
       </c>
@@ -3138,7 +3138,7 @@
       <c r="L8" s="20"/>
       <c r="M8" s="21"/>
     </row>
-    <row r="9" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>163</v>
       </c>
@@ -3175,7 +3175,7 @@
       <c r="L9" s="20"/>
       <c r="M9" s="21"/>
     </row>
-    <row r="10" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>164</v>
       </c>
@@ -3210,7 +3210,7 @@
       <c r="L10" s="20"/>
       <c r="M10" s="21"/>
     </row>
-    <row r="11" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>165</v>
       </c>
@@ -3245,7 +3245,7 @@
       <c r="L11" s="20"/>
       <c r="M11" s="21"/>
     </row>
-    <row r="12" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="11" t="s">
         <v>166</v>
       </c>
@@ -3282,7 +3282,7 @@
       <c r="L12" s="24"/>
       <c r="M12" s="25"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
         <v>167</v>
       </c>
@@ -3314,7 +3314,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
         <v>168</v>
       </c>
@@ -3346,7 +3346,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
         <v>169</v>
       </c>
@@ -3378,7 +3378,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="15" t="s">
         <v>170</v>
       </c>
@@ -3413,7 +3413,7 @@
       <c r="L16" s="26"/>
       <c r="M16" s="27"/>
     </row>
-    <row r="17" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>171</v>
       </c>
@@ -3448,7 +3448,7 @@
       <c r="L17" s="20"/>
       <c r="M17" s="21"/>
     </row>
-    <row r="18" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>172</v>
       </c>
@@ -3483,7 +3483,7 @@
       <c r="L18" s="20"/>
       <c r="M18" s="21"/>
     </row>
-    <row r="19" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>173</v>
       </c>
@@ -3518,7 +3518,7 @@
       <c r="L19" s="20"/>
       <c r="M19" s="21"/>
     </row>
-    <row r="20" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="11" t="s">
         <v>174</v>
       </c>
@@ -3553,7 +3553,7 @@
       </c>
       <c r="M20" s="25"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="8" t="s">
         <v>175</v>
       </c>
@@ -3588,7 +3588,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="8" t="s">
         <v>176</v>
       </c>
@@ -3620,7 +3620,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="8" t="s">
         <v>177</v>
       </c>
@@ -3652,7 +3652,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="8" t="s">
         <v>178</v>
       </c>
@@ -3687,7 +3687,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="8" t="s">
         <v>179</v>
       </c>
@@ -3719,7 +3719,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="15" t="s">
         <v>180</v>
       </c>
@@ -3758,7 +3758,7 @@
       </c>
       <c r="M26" s="27"/>
     </row>
-    <row r="27" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="7" t="s">
         <v>181</v>
       </c>
@@ -3793,7 +3793,7 @@
       <c r="L27" s="20"/>
       <c r="M27" s="21"/>
     </row>
-    <row r="28" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="7" t="s">
         <v>182</v>
       </c>
@@ -3828,7 +3828,7 @@
       <c r="L28" s="20"/>
       <c r="M28" s="21"/>
     </row>
-    <row r="29" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="7" t="s">
         <v>183</v>
       </c>
@@ -3863,7 +3863,7 @@
       </c>
       <c r="M29" s="21"/>
     </row>
-    <row r="30" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="11" t="s">
         <v>184</v>
       </c>
@@ -3912,23 +3912,23 @@
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="2"/>
-    <col min="4" max="4" width="9.140625" style="3"/>
-    <col min="5" max="5" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.140625" style="3"/>
-    <col min="8" max="8" width="9.140625" style="2"/>
-    <col min="9" max="9" width="9.140625" style="3"/>
-    <col min="10" max="10" width="8.5703125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="8.42578125" style="3" customWidth="1"/>
-    <col min="12" max="12" width="25.7109375" style="19" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="22"/>
+    <col min="1" max="1" width="4.453125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7265625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" style="2"/>
+    <col min="4" max="4" width="9.1796875" style="3"/>
+    <col min="5" max="5" width="12.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.1796875" style="3"/>
+    <col min="8" max="8" width="9.1796875" style="2"/>
+    <col min="9" max="9" width="9.1796875" style="3"/>
+    <col min="10" max="10" width="8.54296875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="8.453125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="25.7265625" style="19" customWidth="1"/>
+    <col min="13" max="13" width="9.1796875" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>131</v>
       </c>
@@ -3967,7 +3967,7 @@
       </c>
       <c r="M1" s="25"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>185</v>
       </c>
@@ -3999,7 +3999,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>186</v>
       </c>
@@ -4031,7 +4031,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>187</v>
       </c>
@@ -4063,7 +4063,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>188</v>
       </c>
@@ -4101,7 +4101,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>189</v>
       </c>
@@ -4136,7 +4136,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>190</v>
       </c>
@@ -4171,7 +4171,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
         <v>191</v>
       </c>
@@ -4206,7 +4206,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
         <v>192</v>
       </c>
@@ -4241,7 +4241,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>193</v>
       </c>
@@ -4276,7 +4276,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="15" t="s">
         <v>194</v>
       </c>
@@ -4324,25 +4324,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69278EA8-6F9F-49D4-BBEE-C6F7D2601391}">
   <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="2"/>
-    <col min="4" max="7" width="9.140625" style="3"/>
-    <col min="8" max="8" width="9.140625" style="2"/>
-    <col min="9" max="9" width="9.140625" style="3"/>
-    <col min="10" max="10" width="8.5703125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="8.42578125" style="3" customWidth="1"/>
-    <col min="12" max="12" width="25.7109375" style="19" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="22"/>
+    <col min="1" max="1" width="4.453125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7265625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" style="2"/>
+    <col min="4" max="7" width="9.1796875" style="3"/>
+    <col min="8" max="8" width="9.1796875" style="2"/>
+    <col min="9" max="9" width="9.1796875" style="3"/>
+    <col min="10" max="10" width="8.54296875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="8.453125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="25.7265625" style="19" customWidth="1"/>
+    <col min="13" max="13" width="9.1796875" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>131</v>
       </c>
@@ -4381,7 +4381,7 @@
       </c>
       <c r="M1" s="25"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>200</v>
       </c>
@@ -4413,7 +4413,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>201</v>
       </c>
@@ -4448,7 +4448,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>202</v>
       </c>
@@ -4483,7 +4483,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>203</v>
       </c>
@@ -4518,7 +4518,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>204</v>
       </c>
@@ -4553,7 +4553,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>205</v>
       </c>
@@ -4588,7 +4588,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="15" t="s">
         <v>206</v>
       </c>
@@ -4625,7 +4625,7 @@
       <c r="L8" s="26"/>
       <c r="M8" s="27"/>
     </row>
-    <row r="9" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>207</v>
       </c>
@@ -4660,7 +4660,7 @@
       </c>
       <c r="M9" s="21"/>
     </row>
-    <row r="10" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>208</v>
       </c>
@@ -4695,7 +4695,7 @@
       </c>
       <c r="M10" s="21"/>
     </row>
-    <row r="11" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>209</v>
       </c>
@@ -4732,7 +4732,7 @@
       <c r="L11" s="20"/>
       <c r="M11" s="21"/>
     </row>
-    <row r="12" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>210</v>
       </c>
@@ -4769,7 +4769,7 @@
       <c r="L12" s="20"/>
       <c r="M12" s="21"/>
     </row>
-    <row r="13" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>211</v>
       </c>
@@ -4806,7 +4806,7 @@
       <c r="L13" s="20"/>
       <c r="M13" s="21"/>
     </row>
-    <row r="14" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>212</v>
       </c>
@@ -4843,7 +4843,7 @@
       <c r="L14" s="20"/>
       <c r="M14" s="21"/>
     </row>
-    <row r="15" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="11" t="s">
         <v>213</v>
       </c>
@@ -4880,7 +4880,7 @@
       <c r="L15" s="24"/>
       <c r="M15" s="25"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
         <v>214</v>
       </c>
@@ -4915,7 +4915,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
         <v>215</v>
       </c>
@@ -4950,7 +4950,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
         <v>216</v>
       </c>
@@ -4985,7 +4985,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="8" t="s">
         <v>217</v>
       </c>
@@ -5017,7 +5017,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="15" t="s">
         <v>218</v>
       </c>
@@ -5054,7 +5054,7 @@
       <c r="L20" s="26"/>
       <c r="M20" s="27"/>
     </row>
-    <row r="21" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
         <v>219</v>
       </c>
@@ -5089,7 +5089,7 @@
       </c>
       <c r="M21" s="21"/>
     </row>
-    <row r="22" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>220</v>
       </c>
@@ -5126,7 +5126,7 @@
       <c r="L22" s="20"/>
       <c r="M22" s="21"/>
     </row>
-    <row r="23" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>221</v>
       </c>
@@ -5163,7 +5163,7 @@
       <c r="L23" s="20"/>
       <c r="M23" s="21"/>
     </row>
-    <row r="24" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
         <v>222</v>
       </c>
@@ -5200,7 +5200,7 @@
       <c r="L24" s="20"/>
       <c r="M24" s="21"/>
     </row>
-    <row r="25" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
         <v>223</v>
       </c>
@@ -5237,7 +5237,7 @@
       <c r="L25" s="20"/>
       <c r="M25" s="21"/>
     </row>
-    <row r="26" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
         <v>224</v>
       </c>
@@ -5272,7 +5272,7 @@
       <c r="L26" s="20"/>
       <c r="M26" s="21"/>
     </row>
-    <row r="27" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="7" t="s">
         <v>225</v>
       </c>
@@ -5309,7 +5309,7 @@
       <c r="L27" s="20"/>
       <c r="M27" s="21"/>
     </row>
-    <row r="28" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="7" t="s">
         <v>226</v>
       </c>
@@ -5346,7 +5346,7 @@
       <c r="L28" s="20"/>
       <c r="M28" s="21"/>
     </row>
-    <row r="29" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="11" t="s">
         <v>227</v>
       </c>
@@ -5383,7 +5383,7 @@
       <c r="L29" s="24"/>
       <c r="M29" s="25"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="8" t="s">
         <v>228</v>
       </c>
@@ -5418,7 +5418,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="8" t="s">
         <v>229</v>
       </c>
@@ -5453,7 +5453,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="8" t="s">
         <v>230</v>
       </c>
@@ -5488,7 +5488,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="8" t="s">
         <v>231</v>
       </c>
@@ -5523,7 +5523,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" s="8" t="s">
         <v>232</v>
       </c>
@@ -5558,7 +5558,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="8" t="s">
         <v>233</v>
       </c>
@@ -5590,7 +5590,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" s="8" t="s">
         <v>234</v>
       </c>
@@ -5625,7 +5625,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" s="8" t="s">
         <v>235</v>
       </c>
@@ -5660,7 +5660,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="15" t="s">
         <v>236</v>
       </c>
@@ -5697,7 +5697,7 @@
       <c r="L38" s="26"/>
       <c r="M38" s="27"/>
     </row>
-    <row r="39" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="7" t="s">
         <v>237</v>
       </c>
@@ -5734,7 +5734,7 @@
       <c r="L39" s="20"/>
       <c r="M39" s="21"/>
     </row>
-    <row r="40" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="7" t="s">
         <v>238</v>
       </c>
@@ -5771,7 +5771,7 @@
       </c>
       <c r="M40" s="21"/>
     </row>
-    <row r="41" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="7" t="s">
         <v>239</v>
       </c>
@@ -5808,7 +5808,7 @@
       <c r="L41" s="20"/>
       <c r="M41" s="21"/>
     </row>
-    <row r="42" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="7" t="s">
         <v>240</v>
       </c>
@@ -5845,7 +5845,7 @@
       <c r="L42" s="20"/>
       <c r="M42" s="21"/>
     </row>
-    <row r="43" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43" s="7" t="s">
         <v>241</v>
       </c>
@@ -5880,7 +5880,7 @@
       </c>
       <c r="M43" s="21"/>
     </row>
-    <row r="44" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44" s="7" t="s">
         <v>242</v>
       </c>
@@ -5915,7 +5915,7 @@
       </c>
       <c r="M44" s="21"/>
     </row>
-    <row r="45" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A45" s="11" t="s">
         <v>243</v>
       </c>
@@ -5967,21 +5967,21 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="2"/>
-    <col min="4" max="7" width="9.140625" style="3"/>
-    <col min="8" max="8" width="9.140625" style="2"/>
-    <col min="9" max="9" width="9.140625" style="3"/>
-    <col min="10" max="10" width="8.5703125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="8.42578125" style="3" customWidth="1"/>
-    <col min="12" max="12" width="25.7109375" style="19" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="22"/>
+    <col min="1" max="1" width="3.1796875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7265625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" style="2"/>
+    <col min="4" max="7" width="9.1796875" style="3"/>
+    <col min="8" max="8" width="9.1796875" style="2"/>
+    <col min="9" max="9" width="9.1796875" style="3"/>
+    <col min="10" max="10" width="8.54296875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="8.453125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="25.7265625" style="19" customWidth="1"/>
+    <col min="13" max="13" width="9.1796875" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>131</v>
       </c>
@@ -6020,7 +6020,7 @@
       </c>
       <c r="M1" s="25"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>195</v>
       </c>
@@ -6052,7 +6052,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>199</v>
       </c>
@@ -6084,7 +6084,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>198</v>
       </c>
@@ -6119,7 +6119,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>196</v>
       </c>
@@ -6154,7 +6154,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>244</v>
       </c>
@@ -6186,7 +6186,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>197</v>
       </c>
@@ -6231,22 +6231,22 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="2"/>
-    <col min="4" max="7" width="9.140625" style="3"/>
-    <col min="8" max="8" width="8.5703125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="8.42578125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="25.7109375" style="19" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="22"/>
+    <col min="1" max="1" width="3.1796875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7265625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" style="2"/>
+    <col min="4" max="7" width="9.1796875" style="3"/>
+    <col min="8" max="8" width="8.54296875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="8.453125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="25.7265625" style="19" customWidth="1"/>
+    <col min="11" max="11" width="9.1796875" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>131</v>
       </c>
@@ -6279,7 +6279,7 @@
       </c>
       <c r="K1" s="25"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>256</v>
       </c>
@@ -6302,7 +6302,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>257</v>
       </c>
@@ -6325,7 +6325,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>258</v>
       </c>
@@ -6348,7 +6348,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>259</v>
       </c>
@@ -6371,7 +6371,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>260</v>
       </c>
@@ -6394,7 +6394,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>261</v>
       </c>
@@ -6417,7 +6417,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
         <v>262</v>
       </c>
@@ -6440,7 +6440,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
         <v>263</v>
       </c>
@@ -6463,7 +6463,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>264</v>
       </c>

</xml_diff>

<commit_message>
started implementing the initial population
</commit_message>
<xml_diff>
--- a/scripts/data/__index__.xlsx
+++ b/scripts/data/__index__.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FEBC61-1C44-487D-B64C-5DBBFC95A2F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="notes" sheetId="16" r:id="rId1"/>
@@ -1950,8 +1950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72057042-979B-4A98-BA2E-14DCB6564B56}">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2838,7 +2838,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9578FDA3-F26E-4E35-80A8-9B064AEAD5AE}">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added some helpful features to api
</commit_message>
<xml_diff>
--- a/scripts/data/__index__.xlsx
+++ b/scripts/data/__index__.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FEBC61-1C44-487D-B64C-5DBBFC95A2F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="notes" sheetId="16" r:id="rId1"/>
@@ -1950,8 +1950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72057042-979B-4A98-BA2E-14DCB6564B56}">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>